<commit_message>
use clone in SIMrun to avoid changing object; update documentation
</commit_message>
<xml_diff>
--- a/vignettes/Data/R6_Legacy_compare.xlsx
+++ b/vignettes/Data/R6_Legacy_compare.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10507"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10911"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mneely/LAPK/Development/PM_manual/Data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mneely/LAPK/Development/Pmetrics/vignettes/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C7891B9-D2AF-3545-A079-86F4B8973676}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A2283C9-598A-B24C-BA28-7D0364A43D20}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1100" yWindow="820" windowWidth="28040" windowHeight="17440" activeTab="2" xr2:uid="{97DF5138-9A4B-EF42-87DD-B7FE98165DEC}"/>
   </bookViews>
@@ -102,9 +102,6 @@
     <t>Plot residuals</t>
   </si>
   <si>
-    <t>PM_result$op$plot(resid = T,…)</t>
-  </si>
-  <si>
     <t>plot(op, resid = T)</t>
   </si>
   <si>
@@ -117,9 +114,6 @@
     <t>Construct VPC, pcVPC, NPDE</t>
   </si>
   <si>
-    <t>PM_valid$plot()</t>
-  </si>
-  <si>
     <t>plot(PMvalid)</t>
   </si>
   <si>
@@ -129,9 +123,6 @@
     <t>PMstep()</t>
   </si>
   <si>
-    <t>PM_result$step()</t>
-  </si>
-  <si>
     <t>Calculate AUC</t>
   </si>
   <si>
@@ -169,6 +160,15 @@
   </si>
   <si>
     <t>PM_sim\$pta() or PM_pta\$new()</t>
+  </si>
+  <si>
+    <t>PM_result\$step()</t>
+  </si>
+  <si>
+    <t>PM_valid\$plot()</t>
+  </si>
+  <si>
+    <t>PM_result\$op\$plot(resid = T,…)</t>
   </si>
 </sst>
 </file>
@@ -549,7 +549,7 @@
         <v>3</v>
       </c>
       <c r="B2" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="C2" t="s">
         <v>4</v>
@@ -560,7 +560,7 @@
         <v>5</v>
       </c>
       <c r="B3" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="C3" t="s">
         <v>6</v>
@@ -571,7 +571,7 @@
         <v>7</v>
       </c>
       <c r="B4" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="C4" t="s">
         <v>8</v>
@@ -582,7 +582,7 @@
         <v>9</v>
       </c>
       <c r="B5" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="C5" t="s">
         <v>10</v>
@@ -632,7 +632,7 @@
   <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4:C4"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -669,43 +669,43 @@
         <v>20</v>
       </c>
       <c r="B3" t="s">
+        <v>43</v>
+      </c>
+      <c r="C3" t="s">
         <v>21</v>
-      </c>
-      <c r="C3" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B4" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="C4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B5" t="s">
-        <v>26</v>
+        <v>42</v>
       </c>
       <c r="C5" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B6" t="s">
-        <v>30</v>
+        <v>41</v>
       </c>
       <c r="C6" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
   </sheetData>
@@ -742,35 +742,35 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="B2" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="C2" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="B3" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="C3" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="B4" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="C4" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
     </row>
   </sheetData>

</xml_diff>